<commit_message>
eLearning: en, kr (new)
</commit_message>
<xml_diff>
--- a/eLearning/en/QR/webAddress.xlsx
+++ b/eLearning/en/QR/webAddress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\estat\eLearning\en\QR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B31B0895-0959-4FED-A097-45DB53504DB9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8EDC8B-CB3E-468A-8A7C-957EB3BEBBCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29040" yWindow="210" windowWidth="13710" windowHeight="14670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33570" yWindow="1170" windowWidth="16665" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="330">
   <si>
     <t>estatLecture</t>
   </si>
@@ -1000,6 +1000,21 @@
   </si>
   <si>
     <t>eStatH_65ConfidenceIntervalMuH</t>
+  </si>
+  <si>
+    <t>eStatU_990Friedman</t>
+  </si>
+  <si>
+    <t>eStatU_02LineGraph</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStatU/02LineGraph.htm</t>
+  </si>
+  <si>
+    <t>eStatH_02LineGraph</t>
+  </si>
+  <si>
+    <t>http://www.estat.me/estat/eStatH/02LineGraph.htm</t>
   </si>
 </sst>
 </file>
@@ -1381,10 +1396,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:B169"/>
+  <dimension ref="A1:B173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2026,682 +2041,712 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>233</v>
+      <c r="A84" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>160</v>
+        <v>242</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>190</v>
+        <v>160</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="4" t="s">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B95" s="3" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="3" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="4" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B97" s="3" t="s">
         <v>311</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
-        <v>242</v>
+        <v>268</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>238</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>149</v>
+        <v>242</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B105" s="2" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>154</v>
+        <v>314</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>148</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B140" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B141" s="2" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B142" s="1" t="s">
-        <v>201</v>
-      </c>
+      <c r="A142" s="2"/>
+      <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="B143" s="1" t="s">
-        <v>218</v>
+        <v>200</v>
+      </c>
+      <c r="B143" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>216</v>
+      <c r="A145" s="4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B145" s="5" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B150" s="5" t="s">
-        <v>249</v>
+      <c r="A150" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B150" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B155" s="3" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="4" t="s">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B156" s="3" t="s">
         <v>252</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="B156" s="5" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B159" s="2" t="s">
-        <v>208</v>
+        <v>246</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B162" s="2" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="B161" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="4" t="s">
-        <v>317</v>
-      </c>
-      <c r="B162" s="5" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>210</v>
+        <v>258</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B164" s="2" t="s">
-        <v>211</v>
+        <v>317</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A169" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A170" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B168" s="2" t="s">
+      <c r="B170" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A169" s="4" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A171" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B171" s="3" t="s">
         <v>261</v>
       </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A173" s="2"/>
+      <c r="B173" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2709,43 +2754,45 @@
     <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="B30" r:id="rId4" xr:uid="{F8D7961E-F258-4FA5-869E-615435136B0E}"/>
-    <hyperlink ref="B142" r:id="rId5" xr:uid="{F1887E5F-E1B9-4A84-9B9E-DDC0A791549C}"/>
-    <hyperlink ref="B144" r:id="rId6" xr:uid="{F62620CB-0F76-435D-8F02-4990C6FA6E2F}"/>
-    <hyperlink ref="B145" r:id="rId7" xr:uid="{2D2D479E-2BC8-45DE-AC48-AB3B303F136F}"/>
-    <hyperlink ref="B146" r:id="rId8" xr:uid="{90F3C80F-F3B7-4D66-A216-6EB9BF4687FC}"/>
-    <hyperlink ref="B147" r:id="rId9" xr:uid="{B8BB09CF-5257-4D72-B3DE-AA4ED0D45388}"/>
-    <hyperlink ref="B148" r:id="rId10" xr:uid="{5A3B1D71-7DC4-466D-BD42-9DA4639A6F7C}"/>
-    <hyperlink ref="B149" r:id="rId11" xr:uid="{B4778807-D645-46D7-A508-45CC403C71EB}"/>
-    <hyperlink ref="B158" r:id="rId12" xr:uid="{2C81A0F1-582F-4F81-A78F-31AE9DF53C7E}"/>
-    <hyperlink ref="B143" r:id="rId13" xr:uid="{63A0D520-F036-4E56-A18F-5DF82F89FACB}"/>
-    <hyperlink ref="B151" r:id="rId14" xr:uid="{095D3079-7E54-4AD1-AE13-D731D8402248}"/>
+    <hyperlink ref="B143" r:id="rId5" xr:uid="{F1887E5F-E1B9-4A84-9B9E-DDC0A791549C}"/>
+    <hyperlink ref="B146" r:id="rId6" xr:uid="{F62620CB-0F76-435D-8F02-4990C6FA6E2F}"/>
+    <hyperlink ref="B147" r:id="rId7" xr:uid="{2D2D479E-2BC8-45DE-AC48-AB3B303F136F}"/>
+    <hyperlink ref="B148" r:id="rId8" xr:uid="{90F3C80F-F3B7-4D66-A216-6EB9BF4687FC}"/>
+    <hyperlink ref="B149" r:id="rId9" xr:uid="{B8BB09CF-5257-4D72-B3DE-AA4ED0D45388}"/>
+    <hyperlink ref="B150" r:id="rId10" xr:uid="{5A3B1D71-7DC4-466D-BD42-9DA4639A6F7C}"/>
+    <hyperlink ref="B151" r:id="rId11" xr:uid="{B4778807-D645-46D7-A508-45CC403C71EB}"/>
+    <hyperlink ref="B160" r:id="rId12" xr:uid="{2C81A0F1-582F-4F81-A78F-31AE9DF53C7E}"/>
+    <hyperlink ref="B144" r:id="rId13" xr:uid="{63A0D520-F036-4E56-A18F-5DF82F89FACB}"/>
+    <hyperlink ref="B153" r:id="rId14" xr:uid="{095D3079-7E54-4AD1-AE13-D731D8402248}"/>
     <hyperlink ref="B83" r:id="rId15" xr:uid="{919CEF29-99E8-4D25-842B-D0052EF37549}"/>
-    <hyperlink ref="B84" r:id="rId16" xr:uid="{85376BCA-BA45-4C16-AD62-532F69EFD8EA}"/>
-    <hyperlink ref="B85" r:id="rId17" xr:uid="{11E11649-F346-4B1E-AE28-3F6DC4D3D8E8}"/>
-    <hyperlink ref="B86" r:id="rId18" xr:uid="{A5311A07-65A8-4357-BA1A-2A354D6FF251}"/>
-    <hyperlink ref="B87" r:id="rId19" xr:uid="{01B4AAA8-7F20-4025-9D6A-2AE22F93FE86}"/>
-    <hyperlink ref="B90" r:id="rId20" xr:uid="{6E2305E9-1E44-478C-A2B5-6E0045B27138}"/>
-    <hyperlink ref="B89" r:id="rId21" xr:uid="{B3B97DD5-2F8A-4678-AA58-9A9B84B45533}"/>
-    <hyperlink ref="B88" r:id="rId22" xr:uid="{19194B9C-D192-4CD4-A086-2D07B0E4C368}"/>
-    <hyperlink ref="B152" r:id="rId23" xr:uid="{B95774A2-21EA-4F92-89C1-02D4D4F20EBA}"/>
-    <hyperlink ref="B153" r:id="rId24" xr:uid="{0759E9F1-00A7-4074-9EA8-9926EDFF6CA5}"/>
+    <hyperlink ref="B85" r:id="rId16" xr:uid="{85376BCA-BA45-4C16-AD62-532F69EFD8EA}"/>
+    <hyperlink ref="B86" r:id="rId17" xr:uid="{11E11649-F346-4B1E-AE28-3F6DC4D3D8E8}"/>
+    <hyperlink ref="B87" r:id="rId18" xr:uid="{A5311A07-65A8-4357-BA1A-2A354D6FF251}"/>
+    <hyperlink ref="B88" r:id="rId19" xr:uid="{01B4AAA8-7F20-4025-9D6A-2AE22F93FE86}"/>
+    <hyperlink ref="B91" r:id="rId20" xr:uid="{6E2305E9-1E44-478C-A2B5-6E0045B27138}"/>
+    <hyperlink ref="B90" r:id="rId21" xr:uid="{B3B97DD5-2F8A-4678-AA58-9A9B84B45533}"/>
+    <hyperlink ref="B89" r:id="rId22" xr:uid="{19194B9C-D192-4CD4-A086-2D07B0E4C368}"/>
+    <hyperlink ref="B154" r:id="rId23" xr:uid="{B95774A2-21EA-4F92-89C1-02D4D4F20EBA}"/>
+    <hyperlink ref="B155" r:id="rId24" xr:uid="{0759E9F1-00A7-4074-9EA8-9926EDFF6CA5}"/>
     <hyperlink ref="B37" r:id="rId25" xr:uid="{0A1BE190-6BB3-4CBD-92E3-6DABE17F4F10}"/>
-    <hyperlink ref="B150" r:id="rId26" xr:uid="{154FE7F7-05A4-417B-B244-687F3D037A70}"/>
-    <hyperlink ref="B155" r:id="rId27" xr:uid="{FE4F0135-1084-4045-8993-28F142534BDE}"/>
-    <hyperlink ref="B157" r:id="rId28" xr:uid="{91568A1D-BD0A-4E49-9033-86A448EB56D1}"/>
-    <hyperlink ref="B154" r:id="rId29" xr:uid="{74AA7DD7-FF24-427F-B407-3FFACC069029}"/>
-    <hyperlink ref="B156" r:id="rId30" xr:uid="{CB4D95CF-7AD4-42FF-9892-FA39432ADE0F}"/>
-    <hyperlink ref="B161" r:id="rId31" xr:uid="{873867A2-CD70-43DE-A876-D99571F3337F}"/>
-    <hyperlink ref="B162" r:id="rId32" xr:uid="{CFA513B5-2A6D-4234-9197-DD021758E3E5}"/>
-    <hyperlink ref="B169" r:id="rId33" xr:uid="{7685040B-E92B-46C3-B52A-6521A98E5CF4}"/>
-    <hyperlink ref="B95" r:id="rId34" xr:uid="{D0D78C19-6FF0-4644-86FF-130F1537A1E1}"/>
-    <hyperlink ref="B97" r:id="rId35" xr:uid="{C4184651-E51F-4A62-919F-746AE264531A}"/>
-    <hyperlink ref="B98" r:id="rId36" xr:uid="{51C5A23F-B156-468F-9B14-1F949A3D4F5D}"/>
-    <hyperlink ref="B94" r:id="rId37" xr:uid="{83537CDB-74E4-49AB-A77A-5EF10F621C21}"/>
-    <hyperlink ref="B105" r:id="rId38" xr:uid="{781A8CE8-81F1-4C9E-9BD3-A410728F3F4A}"/>
-    <hyperlink ref="B96" r:id="rId39" xr:uid="{CF13D62F-CBDC-44EC-AD11-5BBDDB6EE60B}"/>
+    <hyperlink ref="B152" r:id="rId26" xr:uid="{154FE7F7-05A4-417B-B244-687F3D037A70}"/>
+    <hyperlink ref="B157" r:id="rId27" xr:uid="{FE4F0135-1084-4045-8993-28F142534BDE}"/>
+    <hyperlink ref="B159" r:id="rId28" xr:uid="{91568A1D-BD0A-4E49-9033-86A448EB56D1}"/>
+    <hyperlink ref="B156" r:id="rId29" xr:uid="{74AA7DD7-FF24-427F-B407-3FFACC069029}"/>
+    <hyperlink ref="B158" r:id="rId30" xr:uid="{CB4D95CF-7AD4-42FF-9892-FA39432ADE0F}"/>
+    <hyperlink ref="B163" r:id="rId31" xr:uid="{873867A2-CD70-43DE-A876-D99571F3337F}"/>
+    <hyperlink ref="B164" r:id="rId32" xr:uid="{CFA513B5-2A6D-4234-9197-DD021758E3E5}"/>
+    <hyperlink ref="B171" r:id="rId33" xr:uid="{7685040B-E92B-46C3-B52A-6521A98E5CF4}"/>
+    <hyperlink ref="B96" r:id="rId34" xr:uid="{D0D78C19-6FF0-4644-86FF-130F1537A1E1}"/>
+    <hyperlink ref="B98" r:id="rId35" xr:uid="{C4184651-E51F-4A62-919F-746AE264531A}"/>
+    <hyperlink ref="B99" r:id="rId36" xr:uid="{51C5A23F-B156-468F-9B14-1F949A3D4F5D}"/>
+    <hyperlink ref="B95" r:id="rId37" xr:uid="{83537CDB-74E4-49AB-A77A-5EF10F621C21}"/>
+    <hyperlink ref="B106" r:id="rId38" xr:uid="{781A8CE8-81F1-4C9E-9BD3-A410728F3F4A}"/>
+    <hyperlink ref="B97" r:id="rId39" xr:uid="{CF13D62F-CBDC-44EC-AD11-5BBDDB6EE60B}"/>
+    <hyperlink ref="B84" r:id="rId40" xr:uid="{296BB1BC-E26C-4F9A-A677-B88C1BAAF5C3}"/>
+    <hyperlink ref="B145" r:id="rId41" xr:uid="{690C20CB-9B4E-40F4-B5DC-E157F006C9D3}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId40"/>
+  <pageSetup paperSize="9" scale="73" fitToHeight="0" orientation="landscape" r:id="rId42"/>
 </worksheet>
 </file>
</xml_diff>